<commit_message>
Update class list import template
- Get rid of blue background formatting on cells to match
  cohort template formatting
- Change use of "Mandatory" to "Required" to match product messaging
- Mark only first name, last name and DoB fields as required to match
  product behaviour. Previously child registration, child postcode,
  parent 1 email and parent 1 phone were all also marked as required.
</commit_message>
<xml_diff>
--- a/app/files/class-list-import-template.xlsx
+++ b/app/files/class-list-import-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs.sharepoint.com/sites/msteams_84b494/Shared Documents/Future vaccinations/Future vaccinations/Design &amp; analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EDB62F4-6A9F-4679-834A-3D7970039639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{2EDB62F4-6A9F-4679-834A-3D7970039639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E552211-5270-4CF8-81D9-0379AB703ECB}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="880" windowWidth="27360" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,22 +65,22 @@
     <t>PARENT_2_PHONE</t>
   </si>
   <si>
-    <t>Mandatory: Free text </t>
-  </si>
-  <si>
-    <t>Mandatory: DD/MM/YYYY</t>
-  </si>
-  <si>
-    <t>Mandatory: valid postcode</t>
-  </si>
-  <si>
-    <t>Mandatory: Email address </t>
-  </si>
-  <si>
-    <t>Mandatory: Phone number, (mobile preferred)</t>
+    <t>Optional: Free text </t>
+  </si>
+  <si>
+    <t>Required: Free text </t>
+  </si>
+  <si>
+    <t>Required: DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>Optional: valid postcode</t>
   </si>
   <si>
     <t>Optional: Email address </t>
+  </si>
+  <si>
+    <t>Optional: Phone number, (mobile preferred)</t>
   </si>
   <si>
     <t>Optional: Phone number (mobile preferred) </t>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,48 +99,66 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0F0F0F"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF215C98"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -149,24 +167,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,78 +523,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C9546C-A2D2-48D3-A8E0-DAEF3ECE39BD}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.1">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -585,15 +605,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <DocType xmlns="80d05917-893e-4a06-bb39-47099b578ffd" xsi:nil="true"/>
@@ -610,6 +621,15 @@
     <TaxCatchAll xmlns="754dda3c-967d-4b24-9bc2-1cc61ceab4bc" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,11 +925,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C876B08D-714B-4BF4-B883-950097757B90}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA4DC00-880E-449F-B2E3-25A12598E9D3}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C876B08D-714B-4BF4-B883-950097757B90}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Add CHILD_YEAR_GROUP field to cohort/class list download templates
</commit_message>
<xml_diff>
--- a/app/files/class-list-import-template.xlsx
+++ b/app/files/class-list-import-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs.sharepoint.com/sites/msteams_84b494/Shared Documents/Future vaccinations/Future vaccinations/Design &amp; analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{2EDB62F4-6A9F-4679-834A-3D7970039639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E552211-5270-4CF8-81D9-0379AB703ECB}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{2EDB62F4-6A9F-4679-834A-3D7970039639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC56AE2F-600A-4A6C-B6A8-927123CB66E0}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="880" windowWidth="27360" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>CHILD_REGISTRATION</t>
   </si>
@@ -50,6 +50,9 @@
     <t>CHILD_DATE_OF_BIRTH</t>
   </si>
   <si>
+    <t>CHILD_YEAR_GROUP</t>
+  </si>
+  <si>
     <t>CHILD_POSTCODE</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
   </si>
   <si>
     <t>Required: DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>Optional: Numeric. When specified, a child's cohort year group will be taken from this value rather than calculated from the date of birth.</t>
   </si>
   <si>
     <t>Optional: valid postcode</t>
@@ -90,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,16 +123,34 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0F0F0F"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0F0F0F"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -163,30 +187,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C9546C-A2D2-48D3-A8E0-DAEF3ECE39BD}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -533,15 +579,16 @@
     <col min="2" max="2" width="22.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="24.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="24.140625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="10" max="10" width="26" style="11" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="20.25" customHeight="1">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -554,7 +601,7 @@
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
@@ -569,34 +616,40 @@
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="45.75" customHeight="1">
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>